<commit_message>
Updated all visuals to be negative and with new format. Next round needs to update narrative and visuals for website, and delete old code
</commit_message>
<xml_diff>
--- a/data/gses_alluc.xlsx
+++ b/data/gses_alluc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanolan\OneDrive\IR_Folder\UCSD_Gaps_git\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanolan\OneDrive\IR_Folder\UCSD_Gaps_Quarto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BF2D6D-08B6-466F-985F-62EF6AC276A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A107A0BE-560E-42B2-BCBE-49AF068C4AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{28558A79-D67E-4D71-A296-A0E1F3ACB6D5}"/>
+    <workbookView xWindow="18729" yWindow="4131" windowWidth="25508" windowHeight="11109" xr2:uid="{28558A79-D67E-4D71-A296-A0E1F3ACB6D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,9 +74,6 @@
     <t>Food Security</t>
   </si>
   <si>
-    <t>San Diego</t>
-  </si>
-  <si>
     <t>All UC</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>Low food security</t>
+  </si>
+  <si>
+    <t>UCSD</t>
   </si>
 </sst>
 </file>
@@ -478,7 +478,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -488,14 +488,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16915550-2D4E-4F40-9C10-B12E78AD8667}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.453125" customWidth="1"/>
     <col min="2" max="2" width="15.26953125" customWidth="1"/>
+    <col min="3" max="3" width="22.6328125" customWidth="1"/>
     <col min="4" max="4" width="16.453125" customWidth="1"/>
     <col min="7" max="7" width="17.1796875" customWidth="1"/>
     <col min="8" max="8" width="20.26953125" customWidth="1"/>
@@ -541,25 +542,25 @@
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2">
         <v>2016</v>
       </c>
       <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="I2">
         <v>3</v>
@@ -573,25 +574,25 @@
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3">
         <v>2016</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -605,25 +606,25 @@
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4">
         <v>2021</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -637,25 +638,25 @@
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5">
         <v>2021</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I5">
         <v>2</v>
@@ -669,25 +670,25 @@
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6">
         <v>2021</v>
       </c>
       <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="I6">
         <v>3</v>
@@ -701,25 +702,25 @@
         <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7">
         <v>2016</v>
       </c>
       <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="I7">
         <v>3</v>
@@ -733,25 +734,25 @@
         <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8">
         <v>2016</v>
       </c>
       <c r="G8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -765,25 +766,25 @@
         <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9">
         <v>2021</v>
       </c>
       <c r="G9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -797,25 +798,25 @@
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F10">
         <v>2021</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I10">
         <v>2</v>
@@ -829,25 +830,25 @@
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11">
         <v>2021</v>
       </c>
       <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="I11">
         <v>3</v>
@@ -857,6 +858,10 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K11">
+    <sortCondition ref="B2:B11"/>
+    <sortCondition ref="F2:F11"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>